<commit_message>
various drug resistance changes
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugResistancePublications.xlsx
+++ b/tabular/drug_resistance/drugResistancePublications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="9980" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="14300" yWindow="12700" windowWidth="32500" windowHeight="9440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -58,16 +58,61 @@
   </si>
   <si>
     <t>http://aac.asm.org/content/54/5/1878.long</t>
+  </si>
+  <si>
+    <t>Lenz_et_al_2013</t>
+  </si>
+  <si>
+    <t>Virologic response and characterisation of HCV genotype 2-6 in patients receiving TMC435 monotherapy (study TMC435-C202)</t>
+  </si>
+  <si>
+    <t>Journal of Hepatology</t>
+  </si>
+  <si>
+    <t>58(3):445-51</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S016882781200829X</t>
+  </si>
+  <si>
+    <t>Lenz O, Vijgen L, Berke JM, Cummings MD, Fevery B, Peeters M, De Smedt G, Moreno C, Picchio G</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>Lenz et al., 2010</t>
+  </si>
+  <si>
+    <t>Lenz et al., 2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,13 +135,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,67 +479,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2010</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2013</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" s="2"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
extra drug publications. initial work to improve drug modelling.
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugResistancePublications.xlsx
+++ b/tabular/drug_resistance/drugResistancePublications.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -103,6 +103,66 @@
   </si>
   <si>
     <t>Lenz O, Verbinnen T, Lin TI, Vijgen L, Cummings MD, Lindberg J, Berke JM, Dehertogh P, Fransen E, Scholliers A, Vermeiren K, Ivens T, Raboisson P, Edlund M, Storm S, Vrang L, de Kock H, Fanning GC, Simmen KA</t>
+  </si>
+  <si>
+    <t>Pawlotsky_2016</t>
+  </si>
+  <si>
+    <t>Pawlotsky, 2016</t>
+  </si>
+  <si>
+    <t>Pawlotsky, J-M</t>
+  </si>
+  <si>
+    <t>Hepatitis C Virus Resistance to Direct-Acting Antiviral Drugs in Interferon-Free Regimens</t>
+  </si>
+  <si>
+    <t>Gastroenterology</t>
+  </si>
+  <si>
+    <t>151(1):70-86</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0016508516300555</t>
+  </si>
+  <si>
+    <t>Sarrazin_2016</t>
+  </si>
+  <si>
+    <t>Sarrazin, 2016</t>
+  </si>
+  <si>
+    <t>Sarrazin, C</t>
+  </si>
+  <si>
+    <t>The importance of resistance to direct antiviral drugs in HCV infection in clinical practice</t>
+  </si>
+  <si>
+    <t>64(2):486-504</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0168827815006297</t>
+  </si>
+  <si>
+    <t>Lontok_et_al_2015</t>
+  </si>
+  <si>
+    <t>Lontok et al., 2015</t>
+  </si>
+  <si>
+    <t>Lontok E, Harrington P, Howe A, Kieffer T, Lennerstrand J, Lenz O, McPhee F, Mo H, Parkin N, Pilot-Matias T, Miller V</t>
+  </si>
+  <si>
+    <t>Hepatitis C virus drug resistance-associated substitutions: State of the art summary</t>
+  </si>
+  <si>
+    <t>Hepatology</t>
+  </si>
+  <si>
+    <t>62(5):1623-32</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.27934/abstract;jsessionid=657E6E3C85196C806137825E68AA9660.f02t01</t>
   </si>
 </sst>
 </file>
@@ -509,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:J4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -626,6 +686,84 @@
         <v>24</v>
       </c>
     </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>2016</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6">
+        <v>2016</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <v>2015</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
improved drug resistance data.
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugResistancePublications.xlsx
+++ b/tabular/drug_resistance/drugResistancePublications.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -42,67 +42,10 @@
     <t>WebLink</t>
   </si>
   <si>
-    <t>Lenz_et_al_2010</t>
-  </si>
-  <si>
-    <t>In vitro resistance profile of the hepatitis C virus NS3/4A protease inhibitor TMC435</t>
-  </si>
-  <si>
-    <t>Antimicrobial Agents and Chemotherapy</t>
-  </si>
-  <si>
-    <t>54(5):1878-87</t>
-  </si>
-  <si>
-    <t>http://aac.asm.org/content/54/5/1878.long</t>
-  </si>
-  <si>
-    <t>Lenz_et_al_2013</t>
-  </si>
-  <si>
-    <t>Virologic response and characterisation of HCV genotype 2-6 in patients receiving TMC435 monotherapy (study TMC435-C202)</t>
-  </si>
-  <si>
     <t>Journal of Hepatology</t>
   </si>
   <si>
-    <t>58(3):445-51</t>
-  </si>
-  <si>
-    <t>http://www.sciencedirect.com/science/article/pii/S016882781200829X</t>
-  </si>
-  <si>
-    <t>Lenz O, Vijgen L, Berke JM, Cummings MD, Fevery B, Peeters M, De Smedt G, Moreno C, Picchio G</t>
-  </si>
-  <si>
     <t>DisplayName</t>
-  </si>
-  <si>
-    <t>Lenz et al., 2010</t>
-  </si>
-  <si>
-    <t>Lenz et al., 2013</t>
-  </si>
-  <si>
-    <t>In vitro and in vivo antiviral activity and resistance profile of the hepatitis C virus NS3/4A protease inhibitor ABT-450</t>
-  </si>
-  <si>
-    <t>Pilot-Matias T, Tripathi R, Cohen D, Gaultier I, Dekhtyar T, Lu L, Reisch T, Irvin M, Hopkins T, Pithawalla R, Middleton T, Ng T, McDaniel K, Or YS, Menon R, Kempf D, Molla A, Collins C</t>
-  </si>
-  <si>
-    <t>59(2):988-97</t>
-  </si>
-  <si>
-    <t>http://aac.asm.org/content/59/2/988.long</t>
-  </si>
-  <si>
-    <t>Pilot_Matias_et_al_2015</t>
-  </si>
-  <si>
-    <t>Pilot-Matias et al., 2015</t>
-  </si>
-  <si>
-    <t>Lenz O, Verbinnen T, Lin TI, Vijgen L, Cummings MD, Lindberg J, Berke JM, Dehertogh P, Fransen E, Scholliers A, Vermeiren K, Ivens T, Raboisson P, Edlund M, Storm S, Vrang L, de Kock H, Fanning GC, Simmen KA</t>
   </si>
   <si>
     <t>Pawlotsky_2016</t>
@@ -569,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -587,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -610,158 +553,80 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2016</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <v>2013</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>2015</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>2016</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6">
-        <v>2016</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7">
-        <v>2015</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated publications / trials.
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugResistancePublications.xlsx
+++ b/tabular/drug_resistance/drugResistancePublications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="9700" windowWidth="32500" windowHeight="9440" tabRatio="500"/>
+    <workbookView xWindow="11340" yWindow="7680" windowWidth="43220" windowHeight="13960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -105,7 +105,271 @@
     <t>62(5):1623-32</t>
   </si>
   <si>
-    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.27934/abstract;jsessionid=657E6E3C85196C806137825E68AA9660.f02t01</t>
+    <t>Lawitz_et_al_2016</t>
+  </si>
+  <si>
+    <t>Lawitz et al., 2016</t>
+  </si>
+  <si>
+    <t>Lawitz E, Matusow G, DeJesus E, Yoshida EM, Felizarta F, Ghalib R, Godofsky E, Herring RW, Poleynard G, Sheikh A, Tobias H, Kugelmas M, Kalmeijer R, Peeters M, Lenz O, Fevery B, De La Rosa G, Scott J, Sinha R and Witek J.</t>
+  </si>
+  <si>
+    <t>Simeprevir plus sofosbuvir in patients with chronic hepatitis C virus genotype 1 infection and cirrhosis: A phase 3 study (OPTIMIST-2)</t>
+  </si>
+  <si>
+    <t>64(2):360-9</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.28422/abstract</t>
+  </si>
+  <si>
+    <t>Foster_et_al_2015</t>
+  </si>
+  <si>
+    <t>Foster et al., 2015</t>
+  </si>
+  <si>
+    <t>Foster GR, Afdhal N, Roberts SK, Bräu N, Gane EJ, Pianko S, Lawitz E, Thompson A, Shiffman ML, Cooper C, Towner WJ, Conway B, Ruane P, Bourlière M, Asselah T, Berg T, Zeuzem S, Rosenberg W, Agarwal K, Stedman CA, Mo H, Dvory-Sobol H, Han L, Wang J, McNally J, Osinusi A, Brainard DM, McHutchison JG, Mazzotta F, Tran TT, Gordon SC, Patel K, Reau N, Mangia A, Sulkowski M; ASTRAL-2 Investigators; ASTRAL-3 Investigators</t>
+  </si>
+  <si>
+    <t>Sofosbuvir and Velpatasvir for HCV Genotype 2 and 3 Infection</t>
+  </si>
+  <si>
+    <t>New England Journal of Medicine</t>
+  </si>
+  <si>
+    <t>373(27):2608-17</t>
+  </si>
+  <si>
+    <t>http://www.nejm.org/doi/full/10.1056/NEJMoa1512612</t>
+  </si>
+  <si>
+    <t>Sulkowski_et_al_2014</t>
+  </si>
+  <si>
+    <t>Poordad_et_al_2016</t>
+  </si>
+  <si>
+    <t>Luetkemeyer_et_al_2016</t>
+  </si>
+  <si>
+    <t>Kwo_et_al_2017</t>
+  </si>
+  <si>
+    <t>Afdhal_et_al_2014a</t>
+  </si>
+  <si>
+    <t>Afdhal_et_al_2014b</t>
+  </si>
+  <si>
+    <t>Kowdley_et_al_2014</t>
+  </si>
+  <si>
+    <t>Naggie_et_al_2015</t>
+  </si>
+  <si>
+    <t>Zeuzem_et_al_2015a</t>
+  </si>
+  <si>
+    <t>Zeuzem_et_al_2015b</t>
+  </si>
+  <si>
+    <t>Nelson_et_al_2015</t>
+  </si>
+  <si>
+    <t>Leroy_et_al_2016</t>
+  </si>
+  <si>
+    <t>Luetkemeyer et al., 2016</t>
+  </si>
+  <si>
+    <t>Kwo et al., 2017</t>
+  </si>
+  <si>
+    <t>Zeuzem et al., 2015a</t>
+  </si>
+  <si>
+    <t>Afdhal et al., 2014a</t>
+  </si>
+  <si>
+    <t>Afdhal et al., 2014b</t>
+  </si>
+  <si>
+    <t>Kowdley et al., 2014</t>
+  </si>
+  <si>
+    <t>Naggie et al., 2015</t>
+  </si>
+  <si>
+    <t>Zeuzem et al., 2015b</t>
+  </si>
+  <si>
+    <t>Nelson et al., 2015</t>
+  </si>
+  <si>
+    <t>Leroy et al., 2016</t>
+  </si>
+  <si>
+    <t>Sulkowski et al., 2014</t>
+  </si>
+  <si>
+    <t>Poordad et al., 2016</t>
+  </si>
+  <si>
+    <t>Sulkowski MS, Gardiner DF, Rodriguez-Torres M, Reddy KR, Hassanein T, Jacobson I, Lawitz E, Lok AS, Hinestrosa F, Thuluvath PJ, Schwartz H, Nelson DR, Everson GT, Eley T, Wind-Rotolo M, Huang SP, Gao M, Hernandez D, McPhee F, Sherman D, Hindes R, Symonds W, Pasquinelli C, Grasela DM; AI444040 Study Group.</t>
+  </si>
+  <si>
+    <t>Daclatasvir plus sofosbuvir for previously treated or untreated chronic HCV infection</t>
+  </si>
+  <si>
+    <t>370(15):1469</t>
+  </si>
+  <si>
+    <t>http://www.nejm.org/doi/full/10.1056/NEJMoa1306218</t>
+  </si>
+  <si>
+    <t>Poordad F, Schiff ER, Vierling JM, Landis C, Fontana RJ, Yang R, McPhee F, Hughes EA, Noviello S, Swenson ES.</t>
+  </si>
+  <si>
+    <t>Daclatasvir with sofosbuvir and ribavirin for hepatitis C virus infection with advanced cirrhosis or post-liver transplantation recurrence</t>
+  </si>
+  <si>
+    <t>63(5):1493-505</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.28446/abstract</t>
+  </si>
+  <si>
+    <t>Luetkemeyer AF, McDonald C, Ramgopal M, Noviello S, Bhore R, Ackerman P.</t>
+  </si>
+  <si>
+    <t>12 Weeks of Daclatasvir in Combination With Sofosbuvir for HIV-HCV Coinfection (ALLY-2 Study): Efficacy and Safety by HIV Combination Antiretroviral Regimens</t>
+  </si>
+  <si>
+    <t>62(12):1489-96</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/cid/article-lookup/doi/10.1093/cid/ciw163</t>
+  </si>
+  <si>
+    <t>Clinical Infectious Diseases</t>
+  </si>
+  <si>
+    <t>Effectiveness of Elbasvir and Grazoprevir Combination, With or Without Ribavirin, for Treatment-Experienced Patients With Chronic Hepatitis C Infection</t>
+  </si>
+  <si>
+    <t>Kwo P, Gane EJ, Peng CY, Pearlman B, Vierling JM, Serfaty L, Buti M, Shafran S, Stryszak P, Lin L, Gress J, Black S, Dutko FJ, Robertson M, Wahl J, Lupinacci L, Barr E, Haber B</t>
+  </si>
+  <si>
+    <t>152(1):164-175</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0016508516351708</t>
+  </si>
+  <si>
+    <t>Grazoprevir-Elbasvir Combination Therapy for Treatment-Naive Cirrhotic and Noncirrhotic Patients With Chronic Hepatitis C Virus Genotype 1, 4, or 6 Infection: A Randomized Trial</t>
+  </si>
+  <si>
+    <t>Zeuzem S, Ghalib R, Reddy KR, Pockros PJ, Ben Ari Z, Zhao Y, Brown DD, Wan S, DiNubile MJ, Nguyen BY, Robertson MN, Wahl J, Barr E, Butterton JR</t>
+  </si>
+  <si>
+    <t>Annals of Internal Medicine</t>
+  </si>
+  <si>
+    <t>163(1):1-13</t>
+  </si>
+  <si>
+    <t>http://annals.org/aim/article/2279766/grazoprevir-elbasvir-combination-therapy-treatment-naive-cirrhotic-noncirrhotic-patients-chronic</t>
+  </si>
+  <si>
+    <t>Ledipasvir and sofosbuvir for untreated HCV genotype 1 infection</t>
+  </si>
+  <si>
+    <t>Afdhal N, Zeuzem S, Kwo P, Chojkier M, Gitlin N, Puoti M, Romero-Gomez M, Zarski JP, Agarwal K, Buggisch P, Foster GR, Bräu N, Buti M, Jacobson IM, Subramanian GM, Ding X, Mo H, Yang JC, Pang PS, Symonds WT, McHutchison JG, Muir AJ, Mangia A, Marcellin P; ION-1 Investigators.</t>
+  </si>
+  <si>
+    <t>http://www.nejm.org/doi/full/10.1056/NEJMoa1402454</t>
+  </si>
+  <si>
+    <t>370(20):1889-98</t>
+  </si>
+  <si>
+    <t>Ledipasvir and sofosbuvir for previously treated HCV genotype 1 infection</t>
+  </si>
+  <si>
+    <t>Afdhal N, Reddy KR, Nelson DR, Lawitz E, Gordon SC, Schiff E, Nahass R, Ghalib R, Gitlin N, Herring R, Lalezari J, Younes ZH, Pockros PJ, Di Bisceglie AM, Arora S, Subramanian GM, Zhu Y, Dvory-Sobol H, Yang JC, Pang PS, Symonds WT, McHutchison JG, Muir AJ, Sulkowski M, Kwo P; ION-2 Investigators.</t>
+  </si>
+  <si>
+    <t>370(16):1483-93</t>
+  </si>
+  <si>
+    <t>http://www.nejm.org/doi/full/10.1056/NEJMoa1316366</t>
+  </si>
+  <si>
+    <t>Ledipasvir and sofosbuvir for 8 or 12 weeks for chronic HCV without cirrhosis</t>
+  </si>
+  <si>
+    <t>Kowdley KV, Gordon SC, Reddy KR, Rossaro L, Bernstein DE, Lawitz E, Shiffman ML, Schiff E, Ghalib R, Ryan M, Rustgi V, Chojkier M, Herring R, Di Bisceglie AM, Pockros PJ, Subramanian GM, An D, Svarovskaia E, Hyland RH, Pang PS, Symonds WT, McHutchison JG, Muir AJ, Pound D, Fried MW; ION-3 Investigators</t>
+  </si>
+  <si>
+    <t>http://www.nejm.org/doi/full/10.1056/NEJMoa1402355</t>
+  </si>
+  <si>
+    <t>370(20):1879-88</t>
+  </si>
+  <si>
+    <t>Ledipasvir and Sofosbuvir for HCV in Patients Coinfected with HIV-1</t>
+  </si>
+  <si>
+    <t>Naggie S, Cooper C, Saag M, Workowski K, Ruane P, Towner WJ, Marks K, Luetkemeyer A, Baden RP, Sax PE, Gane E, Santana-Bagur J, Stamm LM, Yang JC, German P, Dvory-Sobol H, Ni L, Pang PS, McHutchison JG, Stedman CA, Morales-Ramirez JO, Bräu N, Jayaweera D, Colson AE, Tebas P, Wong DK, Dieterich D, Sulkowski M; ION-4 Investigators.</t>
+  </si>
+  <si>
+    <t>http://www.nejm.org/doi/full/10.1056/NEJMoa1501315</t>
+  </si>
+  <si>
+    <t>Prevalence of Pre-Treatment NS5A Resistance Associated Variants in Genotype 1 Patients Across Different Regions Using Deep Sequencing and Effect on Treatment Outcome with LDV/SOF</t>
+  </si>
+  <si>
+    <t>Zeuzem S, Mizokami M, Pianko S, Mangia A, Han KH, Martin R, et al.</t>
+  </si>
+  <si>
+    <t>373(8):705-13</t>
+  </si>
+  <si>
+    <t>62:254A</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.28181/pdf</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.27934/abstract</t>
+  </si>
+  <si>
+    <t>Hepatology 2015</t>
+  </si>
+  <si>
+    <t>All-oral 12-week treatment with daclatasvir plus sofosbuvir in patients with hepatitis C virusgenotype 3 infection: ALLY-3 phase III study</t>
+  </si>
+  <si>
+    <t>Nelson DR, Cooper JN, Lalezari JP, Lawitz E, Pockros PJ, Gitlin N, Freilich BF, Younes ZH, Harlan W, Ghalib R, Oguchi G, Thuluvath PJ, Ortiz-Lasanta G, Rabinovitz M, Bernstein D, Bennett M, Hawkins T, Ravendhran N, Sheikh AM, Varunok P, Kowdley KV, Hennicken D, McPhee F, Rana K, Hughes EA; ALLY-3 Study Team.</t>
+  </si>
+  <si>
+    <t>61(4):1127-35</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.27726/abstract</t>
+  </si>
+  <si>
+    <t>Daclatasvir, sofosbuvir, and ribavirin for hepatitis C virus genotype 3 and advanced liver disease: A randomized phase III study (ALLY-3+)</t>
+  </si>
+  <si>
+    <t>Leroy V, Angus P, Bronowicki JP, Dore GJ, Hezode C, Pianko S, Pol S, Stuart K, Tse E, McPhee F, Bhore R, Jimenez-Exposito MJ, Thompson AJ</t>
+  </si>
+  <si>
+    <t>63(5):1430-41</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1002/hep.28473/abstract</t>
   </si>
 </sst>
 </file>
@@ -164,12 +428,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
@@ -177,12 +462,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,16 +818,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,7 +933,371 @@
         <v>27</v>
       </c>
       <c r="H4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>2016</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>2015</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>2016</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8">
+        <v>2016</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9">
+        <v>2017</v>
+      </c>
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10">
+        <v>2015</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>2014</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>2014</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13">
+        <v>2014</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>2015</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15">
+        <v>2015</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16">
+        <v>2015</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17">
+        <v>2016</v>
+      </c>
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18">
+        <v>2014</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>